<commit_message>
removed old version of the SCMP, updated the schedule spreadsheet and the SPMP, as well as added the unit implementation assignment document
</commit_message>
<xml_diff>
--- a/ProjectDocuments/Java Air - Project Schedule.xlsx
+++ b/ProjectDocuments/Java Air - Project Schedule.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="97">
   <si>
     <t>Plan</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Revise SRS Document Based On Changes</t>
   </si>
   <si>
-    <t>Integrate Source Code with GUI Interfaces</t>
-  </si>
-  <si>
     <t>Develop Source Code for "Customer" Class</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>Develop Source Code for "Data Client" Class</t>
   </si>
   <si>
-    <t>Develop Source Code for "Info Logging" Class</t>
-  </si>
-  <si>
     <t>Develop Source Code for Other Classes</t>
   </si>
   <si>
@@ -333,9 +327,6 @@
     <t>Creation: 9/10/2016</t>
   </si>
   <si>
-    <t>Last Updated: 9/13/2016</t>
-  </si>
-  <si>
     <t>Develop Database ER Diagram</t>
   </si>
   <si>
@@ -400,6 +391,9 @@
   </si>
   <si>
     <t>Review SRS Document With Team</t>
+  </si>
+  <si>
+    <t>Last Updated: 11/4/2016</t>
   </si>
 </sst>
 </file>
@@ -763,7 +757,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -902,14 +896,17 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1427,7 +1424,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="16"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="20"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1437,15 +1434,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>69850</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>31750</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>203200</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>260350</xdr:rowOff>
+          <xdr:rowOff>257175</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1715,45 +1712,48 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BQ68"/>
+  <dimension ref="B2:BQ66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI17" sqref="AI17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" customWidth="1"/>
-    <col min="2" max="2" width="41.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="43.25" style="2" customWidth="1"/>
     <col min="3" max="5" width="7.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.25" style="7" customWidth="1"/>
     <col min="8" max="8" width="4.25" style="1" customWidth="1"/>
-    <col min="9" max="28" width="4.1640625" style="1" customWidth="1"/>
-    <col min="29" max="50" width="4.1640625" customWidth="1"/>
+    <col min="9" max="28" width="4.125" style="1" customWidth="1"/>
+    <col min="29" max="50" width="4.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:69" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="46" t="s">
+    <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="BH2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="AU2" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="AV2" s="49"/>
+      <c r="AW2" s="49"/>
+      <c r="AX2" s="49"/>
+    </row>
+    <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
       <c r="I3" s="8" t="s">
         <v>13</v>
       </c>
@@ -1762,7 +1762,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1789,38 +1789,42 @@
       <c r="AL3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="BH3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
+      <c r="AU3" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV3" s="49"/>
+      <c r="AW3" s="49"/>
+      <c r="AX3" s="49"/>
+    </row>
+    <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
       <c r="AT4" s="1"/>
-      <c r="AU4" s="1"/>
-      <c r="AV4" s="1"/>
-      <c r="AW4" s="1"/>
-      <c r="AX4" s="1"/>
-      <c r="BH4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.4">
+      <c r="AU4" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV4" s="49"/>
+      <c r="AW4" s="49"/>
+      <c r="AX4" s="49"/>
+      <c r="AY4" s="49"/>
+      <c r="AZ4" s="49"/>
+    </row>
+    <row r="5" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="T5" s="34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
     </row>
-    <row r="6" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
@@ -1828,16 +1832,16 @@
       </c>
       <c r="J6" s="4"/>
       <c r="T6" s="39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AF6" s="35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AT6" s="1"/>
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
@@ -1845,62 +1849,62 @@
       </c>
       <c r="J7" s="33"/>
       <c r="K7" s="34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L7" s="34"/>
       <c r="M7" s="34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N7" s="34"/>
       <c r="O7" s="34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P7" s="34"/>
       <c r="Q7" s="34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R7" s="34"/>
       <c r="S7" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T7" s="34"/>
       <c r="U7" s="34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V7" s="34"/>
       <c r="W7" s="34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="X7" s="34"/>
       <c r="Y7" s="34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Z7" s="34"/>
       <c r="AA7" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AB7" s="34"/>
       <c r="AC7" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AD7" s="35"/>
       <c r="AE7" s="35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AF7" s="35"/>
       <c r="AG7" s="35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH7" s="35"/>
       <c r="AI7" s="35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ7" s="35"/>
       <c r="AK7" s="35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="2:69" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="2:69" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="21"/>
       <c r="C8" s="4" t="s">
         <v>2</v>
@@ -2006,7 +2010,7 @@
         <v>42714</v>
       </c>
     </row>
-    <row r="9" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
@@ -2031,7 +2035,7 @@
       </c>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -2161,9 +2165,9 @@
       <c r="BP10" s="3"/>
       <c r="BQ10" s="1"/>
     </row>
-    <row r="11" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I11" s="41"/>
       <c r="J11" s="41"/>
@@ -2194,7 +2198,7 @@
       <c r="AI11" s="41"/>
       <c r="AJ11" s="41"/>
     </row>
-    <row r="12" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
         <v>15</v>
       </c>
@@ -2204,7 +2208,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="17"/>
       <c r="I12" s="45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J12" s="41"/>
       <c r="K12" s="41"/>
@@ -2234,9 +2238,9 @@
       <c r="AI12" s="41"/>
       <c r="AJ12" s="41"/>
     </row>
-    <row r="13" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -2248,7 +2252,7 @@
       <c r="K13" s="41"/>
       <c r="L13" s="41"/>
       <c r="M13" s="45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N13" s="41"/>
       <c r="O13" s="41"/>
@@ -2274,9 +2278,9 @@
       <c r="AI13" s="41"/>
       <c r="AJ13" s="41"/>
     </row>
-    <row r="14" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
@@ -2292,7 +2296,7 @@
       <c r="O14" s="41"/>
       <c r="P14" s="41"/>
       <c r="Q14" s="45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="R14" s="41"/>
       <c r="S14" s="41"/>
@@ -2314,9 +2318,9 @@
       <c r="AI14" s="41"/>
       <c r="AJ14" s="41"/>
     </row>
-    <row r="15" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -2339,7 +2343,7 @@
       <c r="V15" s="41"/>
       <c r="W15" s="41"/>
       <c r="X15" s="45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Y15" s="41"/>
       <c r="Z15" s="41"/>
@@ -2354,9 +2358,9 @@
       <c r="AI15" s="41"/>
       <c r="AJ15" s="41"/>
     </row>
-    <row r="16" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -2379,7 +2383,7 @@
       <c r="W16" s="41"/>
       <c r="X16" s="41"/>
       <c r="Y16" s="45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Z16" s="41"/>
       <c r="AA16" s="41"/>
@@ -2393,9 +2397,9 @@
       <c r="AI16" s="41"/>
       <c r="AJ16" s="41"/>
     </row>
-    <row r="17" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -2420,7 +2424,7 @@
       <c r="X17" s="45"/>
       <c r="Y17" s="41"/>
       <c r="Z17" s="45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AA17" s="41"/>
       <c r="AB17" s="41"/>
@@ -2433,9 +2437,9 @@
       <c r="AI17" s="41"/>
       <c r="AJ17" s="41"/>
     </row>
-    <row r="18" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -2461,10 +2465,9 @@
       <c r="Y18" s="41"/>
       <c r="Z18" s="41"/>
       <c r="AA18" s="41"/>
-      <c r="AB18" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC18" s="41"/>
+      <c r="AC18" s="45" t="s">
+        <v>90</v>
+      </c>
       <c r="AD18" s="41"/>
       <c r="AE18" s="41"/>
       <c r="AF18" s="41"/>
@@ -2473,9 +2476,9 @@
       <c r="AI18" s="41"/>
       <c r="AJ18" s="41"/>
     </row>
-    <row r="19" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -2505,7 +2508,7 @@
       <c r="AC19" s="41"/>
       <c r="AD19" s="45"/>
       <c r="AE19" s="45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AF19" s="41"/>
       <c r="AG19" s="41"/>
@@ -2513,9 +2516,9 @@
       <c r="AI19" s="41"/>
       <c r="AJ19" s="41"/>
     </row>
-    <row r="20" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -2549,11 +2552,11 @@
       <c r="AG20" s="41"/>
       <c r="AH20" s="41"/>
       <c r="AI20" s="45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AJ20" s="41"/>
     </row>
-    <row r="21" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -2589,7 +2592,7 @@
       <c r="AI21" s="41"/>
       <c r="AJ21" s="41"/>
     </row>
-    <row r="22" spans="2:36" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:36" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="22" t="s">
         <v>18</v>
       </c>
@@ -2599,7 +2602,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="s">
         <v>22</v>
       </c>
@@ -2619,9 +2622,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24" s="16">
         <v>5</v>
@@ -2633,13 +2636,13 @@
         <v>4</v>
       </c>
       <c r="F24" s="18">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G24" s="17">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
         <v>23</v>
       </c>
@@ -2653,15 +2656,15 @@
         <v>4</v>
       </c>
       <c r="F25" s="18">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G25" s="17">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="26" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" s="16">
         <v>13</v>
@@ -2672,16 +2675,16 @@
       <c r="E26" s="18">
         <v>17</v>
       </c>
-      <c r="F26" s="18" t="s">
-        <v>42</v>
+      <c r="F26" s="18">
+        <v>1</v>
       </c>
       <c r="G26" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C27" s="16">
         <v>14</v>
@@ -2689,19 +2692,19 @@
       <c r="D27" s="16">
         <v>2</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>42</v>
+      <c r="E27" s="18">
+        <v>17</v>
+      </c>
+      <c r="F27" s="18">
+        <v>1</v>
       </c>
       <c r="G27" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" s="16">
         <v>15</v>
@@ -2710,16 +2713,16 @@
         <v>2</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G28" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="15"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
@@ -2727,7 +2730,7 @@
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
     </row>
-    <row r="30" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
         <v>19</v>
       </c>
@@ -2737,7 +2740,7 @@
       <c r="F30" s="16"/>
       <c r="G30" s="17"/>
     </row>
-    <row r="31" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="s">
         <v>24</v>
       </c>
@@ -2757,9 +2760,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:36" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:36" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C32" s="16">
         <v>6</v>
@@ -2777,7 +2780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="15" t="s">
         <v>32</v>
       </c>
@@ -2794,10 +2797,10 @@
         <v>11</v>
       </c>
       <c r="G33" s="17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="15"/>
       <c r="C34" s="16"/>
       <c r="D34" s="16"/>
@@ -2805,9 +2808,9 @@
       <c r="F34" s="16"/>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="16"/>
@@ -2815,7 +2818,7 @@
       <c r="F35" s="16"/>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="15" t="s">
         <v>31</v>
       </c>
@@ -2835,9 +2838,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C37" s="16">
         <v>5</v>
@@ -2855,9 +2858,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" s="16">
         <v>7</v>
@@ -2875,9 +2878,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C39" s="16">
         <v>12</v>
@@ -2892,12 +2895,12 @@
         <v>1</v>
       </c>
       <c r="G39" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C40" s="16">
         <v>12</v>
@@ -2909,15 +2912,15 @@
         <v>11</v>
       </c>
       <c r="F40" s="18">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G40" s="17">
         <v>0.7</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C41" s="16">
         <v>22</v>
@@ -2926,16 +2929,16 @@
         <v>7</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G41" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="15"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -2943,9 +2946,9 @@
       <c r="F42" s="18"/>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -2953,9 +2956,9 @@
       <c r="F43" s="16"/>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C44" s="16">
         <v>5</v>
@@ -2970,10 +2973,10 @@
         <v>9</v>
       </c>
       <c r="G44" s="17">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="15" t="s">
         <v>30</v>
       </c>
@@ -2990,12 +2993,12 @@
         <v>9</v>
       </c>
       <c r="G45" s="17">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C46" s="16">
         <v>14</v>
@@ -3007,15 +3010,15 @@
         <v>14</v>
       </c>
       <c r="F46" s="18">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G46" s="17">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C47" s="16">
         <v>16</v>
@@ -3033,171 +3036,171 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="15" t="s">
-        <v>33</v>
+    <row r="48" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="C48" s="16">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D48" s="16">
         <v>6</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G48" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="16">
-        <v>23</v>
-      </c>
-      <c r="D49" s="16">
-        <v>6</v>
-      </c>
-      <c r="E49" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F49" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G49" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="15"/>
+    <row r="49" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="15"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+    </row>
+    <row r="50" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="C50" s="16"/>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
     </row>
-    <row r="51" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-    </row>
-    <row r="52" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="16">
+        <v>3</v>
+      </c>
+      <c r="D51" s="16">
+        <v>10</v>
+      </c>
+      <c r="E51" s="16">
+        <v>3</v>
+      </c>
+      <c r="F51" s="18">
+        <v>10</v>
+      </c>
+      <c r="G51" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C52" s="16">
-        <v>3</v>
+        <v>25</v>
+      </c>
+      <c r="C52" s="18">
+        <v>5</v>
       </c>
       <c r="D52" s="16">
-        <v>10</v>
-      </c>
-      <c r="E52" s="16">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="E52" s="18">
+        <v>8</v>
       </c>
       <c r="F52" s="18">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G52" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C53" s="18">
         <v>5</v>
       </c>
       <c r="D53" s="16">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E53" s="18">
         <v>8</v>
       </c>
       <c r="F53" s="18">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G53" s="17">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C54" s="18">
+        <v>27</v>
+      </c>
+      <c r="C54" s="46">
         <v>5</v>
       </c>
-      <c r="D54" s="16">
-        <v>20</v>
+      <c r="D54" s="46">
+        <v>23</v>
       </c>
       <c r="E54" s="18">
+        <v>15</v>
+      </c>
+      <c r="F54" s="18">
         <v>8</v>
       </c>
-      <c r="F54" s="18">
-        <v>10</v>
-      </c>
       <c r="G54" s="17">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C55" s="48">
-        <v>5</v>
-      </c>
-      <c r="D55" s="48">
-        <v>23</v>
+        <v>67</v>
+      </c>
+      <c r="C55" s="46">
+        <v>21</v>
+      </c>
+      <c r="D55" s="46">
+        <v>7</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G55" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" s="48">
+    <row r="56" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="15"/>
+    </row>
+    <row r="57" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D56" s="48">
-        <v>7</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F56" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G56" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B57" s="15"/>
-    </row>
-    <row r="58" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="58" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="16">
+        <v>9</v>
+      </c>
+      <c r="D58" s="16">
+        <v>5</v>
+      </c>
+      <c r="E58" s="18">
+        <v>18</v>
+      </c>
+      <c r="F58" s="18">
+        <v>4</v>
+      </c>
+      <c r="G58" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C59" s="16">
         <v>9</v>
@@ -3205,45 +3208,45 @@
       <c r="D59" s="16">
         <v>5</v>
       </c>
-      <c r="E59" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F59" s="18" t="s">
-        <v>42</v>
+      <c r="E59" s="18">
+        <v>18</v>
+      </c>
+      <c r="F59" s="18">
+        <v>4</v>
       </c>
       <c r="G59" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60" s="16">
+        <v>58</v>
+      </c>
+      <c r="C60" s="18">
         <v>9</v>
       </c>
       <c r="D60" s="16">
-        <v>5</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F60" s="18" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="E60" s="18">
+        <v>14</v>
+      </c>
+      <c r="F60" s="18">
+        <v>8</v>
       </c>
       <c r="G60" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="15" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C61" s="18">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D61" s="16">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E61" s="18">
         <v>14</v>
@@ -3252,10 +3255,10 @@
         <v>4</v>
       </c>
       <c r="G61" s="17">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="15" t="s">
         <v>34</v>
       </c>
@@ -3266,16 +3269,16 @@
         <v>10</v>
       </c>
       <c r="E62" s="18">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F62" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G62" s="17">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="15" t="s">
         <v>35</v>
       </c>
@@ -3285,17 +3288,17 @@
       <c r="D63" s="16">
         <v>10</v>
       </c>
-      <c r="E63" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F63" s="18" t="s">
-        <v>42</v>
+      <c r="E63" s="18">
+        <v>17</v>
+      </c>
+      <c r="F63" s="18">
+        <v>5</v>
       </c>
       <c r="G63" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="15" t="s">
         <v>36</v>
       </c>
@@ -3305,17 +3308,17 @@
       <c r="D64" s="16">
         <v>10</v>
       </c>
-      <c r="E64" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F64" s="18" t="s">
-        <v>42</v>
+      <c r="E64" s="18">
+        <v>17</v>
+      </c>
+      <c r="F64" s="18">
+        <v>5</v>
       </c>
       <c r="G64" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="15" t="s">
         <v>37</v>
       </c>
@@ -3325,81 +3328,44 @@
       <c r="D65" s="16">
         <v>10</v>
       </c>
-      <c r="E65" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F65" s="18" t="s">
-        <v>42</v>
+      <c r="E65" s="18">
+        <v>17</v>
+      </c>
+      <c r="F65" s="18">
+        <v>5</v>
       </c>
       <c r="G65" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="15" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="C66" s="18">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D66" s="16">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G66" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B67" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C67" s="18">
-        <v>13</v>
-      </c>
-      <c r="D67" s="16">
-        <v>10</v>
-      </c>
-      <c r="E67" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F67" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G67" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C68" s="18">
-        <v>23</v>
-      </c>
-      <c r="D68" s="16">
-        <v>5</v>
-      </c>
-      <c r="E68" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F68" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G68" s="17">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="B2:G4"/>
+    <mergeCell ref="AU2:AX2"/>
+    <mergeCell ref="AU3:AX3"/>
+    <mergeCell ref="AU4:AZ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I16:S16 W16:X16 U16 I11:BP15 Z16:BP16 I17:BP68">
+  <conditionalFormatting sqref="I16:S16 W16:X16 U16 I11:BP15 Z16:BP16 I17:BP17 AD18:BP18 I18:AA18 I19:BP66">
     <cfRule type="expression" dxfId="33" priority="17">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3425,7 +3391,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69:BP69">
+  <conditionalFormatting sqref="B67:BP67">
     <cfRule type="expression" dxfId="25" priority="18">
       <formula>TRUE</formula>
     </cfRule>
@@ -3436,59 +3402,85 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16">
-    <cfRule type="expression" dxfId="15" priority="37">
+    <cfRule type="expression" dxfId="23" priority="37">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="38">
+    <cfRule type="expression" dxfId="22" priority="38">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="39">
+    <cfRule type="expression" dxfId="21" priority="39">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="40">
+    <cfRule type="expression" dxfId="20" priority="40">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="41">
+    <cfRule type="expression" dxfId="19" priority="41">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="42">
+    <cfRule type="expression" dxfId="18" priority="42">
       <formula>V$10=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="43">
+    <cfRule type="expression" dxfId="17" priority="43">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="44">
+    <cfRule type="expression" dxfId="16" priority="44">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y16">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>AA$10=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="46" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <conditionalFormatting sqref="AC18">
+    <cfRule type="expression" dxfId="7" priority="53">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="54">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="55">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="56">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="57">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="58">
+      <formula>AB$10=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="59">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="60">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3501,15 +3493,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>14</xdr:col>
-                    <xdr:colOff>69850</xdr:colOff>
+                    <xdr:colOff>66675</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>31750</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>14</xdr:col>
-                    <xdr:colOff>203200</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>260350</xdr:rowOff>
+                    <xdr:rowOff>257175</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3535,29 +3527,29 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.6640625" style="41"/>
-    <col min="4" max="4" width="34.83203125" style="41" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="41"/>
+    <col min="1" max="3" width="8.625" style="41"/>
+    <col min="4" max="4" width="34.875" style="41" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E1" s="42"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43">
         <v>42625</v>
       </c>
@@ -3565,13 +3557,13 @@
         <v>0.1</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43">
         <v>42646</v>
       </c>
@@ -3579,10 +3571,10 @@
         <v>0.2</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>